<commit_message>
Removed RG and DECANT edge cases to simplify.
</commit_message>
<xml_diff>
--- a/Data/RAWDATA_Ward_Scenarios.xlsx
+++ b/Data/RAWDATA_Ward_Scenarios.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oliverlambson/Google Drive/ISMM/Dissertation/2. Scenario Planning/0. WORK/Tactical Tool/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oliverlambson/GitHub/ISMM/CUH_covid_tactical_tool/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91B6C2AC-9808-9A4D-AF7C-3761BC177701}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{077834BB-E7E7-B245-9EFF-AC6C5F838DA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4700" yWindow="3260" windowWidth="27240" windowHeight="16440" xr2:uid="{53D501AF-7FFC-3549-9052-BE3C0FC1A275}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="101">
   <si>
     <t>ATC</t>
   </si>
@@ -197,9 +197,6 @@
     <t>ADD C5</t>
   </si>
   <si>
-    <t>RG</t>
-  </si>
-  <si>
     <t>ADD D5</t>
   </si>
   <si>
@@ -228,9 +225,6 @@
   </si>
   <si>
     <t>ADD D8</t>
-  </si>
-  <si>
-    <t>DECANT</t>
   </si>
   <si>
     <t>DECANT ward (fire safety works)</t>
@@ -518,14 +512,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <fill>
         <patternFill>
@@ -911,44 +898,44 @@
   <dimension ref="A1:K48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:11" ht="17" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -1824,7 +1811,7 @@
         <v>23</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>54</v>
+        <v>6</v>
       </c>
       <c r="F27" s="11">
         <v>23</v>
@@ -1850,7 +1837,7 @@
         <v>46</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>5</v>
@@ -1885,7 +1872,7 @@
         <v>46</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>5</v>
@@ -1920,7 +1907,7 @@
         <v>46</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>5</v>
@@ -1947,7 +1934,7 @@
         <v>27</v>
       </c>
       <c r="K30" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -1955,7 +1942,7 @@
         <v>46</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>5</v>
@@ -1982,7 +1969,7 @@
         <v>23</v>
       </c>
       <c r="K31" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -1990,7 +1977,7 @@
         <v>46</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>5</v>
@@ -2025,7 +2012,7 @@
         <v>46</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>5</v>
@@ -2052,7 +2039,7 @@
         <v>19</v>
       </c>
       <c r="K33" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -2060,7 +2047,7 @@
         <v>46</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>5</v>
@@ -2069,7 +2056,7 @@
         <v>36</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>65</v>
+        <v>6</v>
       </c>
       <c r="F34" s="11">
         <v>0</v>
@@ -2087,7 +2074,7 @@
         <v>15</v>
       </c>
       <c r="K34" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -2095,7 +2082,7 @@
         <v>46</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>5</v>
@@ -2122,7 +2109,7 @@
         <v>5</v>
       </c>
       <c r="K35" s="12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -2130,7 +2117,7 @@
         <v>46</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>5</v>
@@ -2157,7 +2144,7 @@
         <v>13</v>
       </c>
       <c r="K36" s="12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:11">
@@ -2165,7 +2152,7 @@
         <v>46</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>5</v>
@@ -2192,7 +2179,7 @@
         <v>9</v>
       </c>
       <c r="K37" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:11">
@@ -2200,7 +2187,7 @@
         <v>46</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C38" s="13" t="s">
         <v>5</v>
@@ -2232,10 +2219,10 @@
     </row>
     <row r="39" spans="1:11">
       <c r="A39" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>32</v>
@@ -2262,18 +2249,18 @@
         <v>0</v>
       </c>
       <c r="K39" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="40" spans="1:11">
       <c r="A40" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D40" s="18">
         <v>0</v>
@@ -2300,10 +2287,10 @@
     </row>
     <row r="41" spans="1:11">
       <c r="A41" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>5</v>
@@ -2330,15 +2317,15 @@
         <v>18</v>
       </c>
       <c r="K41" s="12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="42" spans="1:11">
       <c r="A42" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C42" s="13" t="s">
         <v>5</v>
@@ -2365,7 +2352,7 @@
         <v>26</v>
       </c>
       <c r="K42" s="17" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="43" spans="1:11">
@@ -2373,7 +2360,7 @@
         <v>10</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>5</v>
@@ -2400,7 +2387,7 @@
         <v>14</v>
       </c>
       <c r="K43" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="44" spans="1:11">
@@ -2408,7 +2395,7 @@
         <v>10</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C44" s="13" t="s">
         <v>5</v>
@@ -2435,7 +2422,7 @@
         <v>26</v>
       </c>
       <c r="K44" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="45" spans="1:11">
@@ -2443,7 +2430,7 @@
         <v>21</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>28</v>
@@ -2476,7 +2463,7 @@
         <v>21</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>5</v>
@@ -2503,7 +2490,7 @@
         <v>8</v>
       </c>
       <c r="K46" s="12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="47" spans="1:11">
@@ -2511,7 +2498,7 @@
         <v>21</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>5</v>
@@ -2538,7 +2525,7 @@
         <v>26</v>
       </c>
       <c r="K47" s="12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="48" spans="1:11">
@@ -2546,7 +2533,7 @@
         <v>21</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C48" s="13" t="s">
         <v>5</v>
@@ -2573,41 +2560,41 @@
         <v>28</v>
       </c>
       <c r="K48" s="17" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E3:E48 G3:G48 I3:I48">
-    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
       <formula>"DECANT"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
       <formula>"RG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
       <formula>"G"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="10" operator="equal">
       <formula>"A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="11" operator="equal">
       <formula>"R"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E4 G2:G4 I2:I4">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"DECANT"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"RG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"G"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
       <formula>"A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
       <formula>"R"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>